<commit_message>
calorimetry : GUI : backend : WIP
</commit_message>
<xml_diff>
--- a/input/calorimetry/ds.2.dsc/data.xlsx
+++ b/input/calorimetry/ds.2.dsc/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="input_k_constants_log10" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t xml:space="preserve">lg_k</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t xml:space="preserve">deviation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MF3H</t>
   </si>
   <si>
     <t xml:space="preserve">name</t>
@@ -187,7 +184,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+      <selection pane="topLeft" activeCell="E14" activeCellId="1" sqref="B1 E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -224,7 +221,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L19" activeCellId="0" sqref="L19"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="B1 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -425,7 +422,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="B1 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -483,8 +480,8 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="1" sqref="B1 B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -822,8 +819,8 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -831,15 +828,15 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.53"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>15</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -872,7 +869,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="B1 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -882,10 +879,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>